<commit_message>
Update table with new test results
</commit_message>
<xml_diff>
--- a/analysis_nist_pqc_signatures.xlsx
+++ b/analysis_nist_pqc_signatures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gilbertndollanedione/Desktop/nist-pqc-first-round-signatures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F492C45E-2296-ED49-A2DA-E9562967291B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38C81A9-E756-BC41-8031-CF831DDAE2B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{C8054BE3-D351-A644-8250-379CA416B869}"/>
   </bookViews>
@@ -8352,6 +8352,194 @@
         <color rgb="FF00B050"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
+      <t>NVI:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">  For the moment, maybe constant time.  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>meas:    0.40 M (M=1e4), max t:   +1.77</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>max tau: 2.78e-03, (5/tau)^2: 3.24e+06.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">                              For the moment, maybe constant time.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                     </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>meas:    0.25 M (M=10.000), max t:   +1.61</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, max tau: 3.24e-03, (5/tau)^2: 2.38e+06. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> NVI:  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>For the moment, maybe constant time.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>meas:    0.24 M (1e4), max t:   +1.37,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">max tau: 2.81e-03, (5/tau)^2: 3.17e+06.  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">       NV: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">Probably not constant time. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>meas:    1.19 M (M=1e5), max t:  +10.32</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">max tau: 9.46e-03, (5/tau)^2: 2.80e+05. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
       <t xml:space="preserve">NVI: </t>
     </r>
     <r>
@@ -8361,6 +8549,276 @@
         <color rgb="FF7030A0"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
+      <t>Probably not constant time.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>meas:    0.84 M (M=1e4), max t:  +10.06,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">max tau: 1.10e-02, (5/tau)^2: 2.08e+05. . </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">     NV:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> Probably not constant time.   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>meas:    0.28 M (M=1e6/1e5/1e3), max t:  +11.01,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">max tau: 2.08e-02, (5/tau)^2: 5.80e+04.  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>NVI:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Definitely</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> not constant time.   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">meas:    0.01 M (M=1e4), max t: +4143.72, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">max tau: 3.67e+01, (5/tau)^2: 1.85e-02. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> Probably not constant time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>meas:    0.01 M (M=1e6)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">,                      </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>max t:  +65.97</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">,           max tau: 6.32e-01, (5/tau)^2: 6.25e+01. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> NVIN: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>For the moment, maybe constant time.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>meas:    0.04 M (M=1e3), max t:   +1.08,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">max tau: 5.27e-03, (5/tau)^2: 8.99e+05.  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">                        NVI: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
       <t>For the moment, maybe constant time</t>
     </r>
     <r>
@@ -8445,413 +8903,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">, max tau: 7.31e-03, (5/tau)^2: 4.68e+05. </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>NVI:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve">  For the moment, maybe constant time.  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>meas:    0.40 M (M=1e4), max t:   +1.77</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>max tau: 2.78e-03, (5/tau)^2: 3.24e+06.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve">                              For the moment, maybe constant time.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                     </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>meas:    0.25 M (M=10.000), max t:   +1.61</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, max tau: 3.24e-03, (5/tau)^2: 2.38e+06. </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve"> NVI:  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>For the moment, maybe constant time.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>meas:    0.24 M (1e4), max t:   +1.37,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve">max tau: 2.81e-03, (5/tau)^2: 3.17e+06.  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve">       NV: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve">Probably not constant time. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>meas:    1.19 M (M=1e5), max t:  +10.32</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve">max tau: 9.46e-03, (5/tau)^2: 2.80e+05. </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve">NVI: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>Probably not constant time.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>meas:    0.84 M (M=1e4), max t:  +10.06,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve">max tau: 1.10e-02, (5/tau)^2: 2.08e+05. . </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve">     NV:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve"> Probably not constant time.   </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>meas:    0.28 M (M=1e6/1e5/1e3), max t:  +11.01,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve">max tau: 2.08e-02, (5/tau)^2: 5.80e+04.  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>NVI:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>Definitely</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve"> not constant time.   </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve">meas:    0.01 M (M=1e4), max t: +4143.72, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve">max tau: 3.67e+01, (5/tau)^2: 1.85e-02. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve"> Probably not constant time</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>meas:    0.01 M (M=1e6)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">,                      </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>max t:  +65.97</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">,           max tau: 6.32e-01, (5/tau)^2: 6.25e+01. </t>
     </r>
   </si>
 </sst>
@@ -9899,8 +9950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36623FBA-CEA1-594C-B41A-AB27154FBA5D}">
   <dimension ref="A1:Q143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B100" zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
-      <selection activeCell="I109" sqref="I109:I113"/>
+    <sheetView tabSelected="1" zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10369,7 +10420,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="51" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="J19" s="22" t="s">
         <v>16</v>
@@ -10547,7 +10598,7 @@
         <v>143</v>
       </c>
       <c r="I27" s="51" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J27" s="55" t="s">
         <v>22</v>
@@ -11362,7 +11413,7 @@
         <v>154</v>
       </c>
       <c r="I62" s="102" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J62" s="25" t="s">
         <v>16</v>
@@ -12481,7 +12532,7 @@
         <v>134</v>
       </c>
       <c r="I109" s="51" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J109" s="70" t="s">
         <v>69</v>
@@ -12604,7 +12655,7 @@
         <v>132</v>
       </c>
       <c r="I114" s="51" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J114" s="25" t="s">
         <v>16</v>

</xml_diff>